<commit_message>
Added test case for cell with pre-existing data in abstract / doi.
</commit_message>
<xml_diff>
--- a/abstract_doi_finder/input/test_input.xlsx
+++ b/abstract_doi_finder/input/test_input.xlsx
@@ -14,6 +14,7 @@
     <sheet name="TR1.csv" sheetId="5" r:id="rId5"/>
     <sheet name="TR1da.csv" sheetId="6" r:id="rId6"/>
     <sheet name="TR1DA.csv(2)" sheetId="7" r:id="rId7"/>
+    <sheet name="TRm.csv" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"m_Presentation.csv"</definedName>
@@ -30,6 +31,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="5">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="6">"TR1DA.csv(2)"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="7">"TRm.csv"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">#REF!</definedName>
   </definedNames>
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" characterSet="UTF-8"/>
@@ -238,8 +241,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Authors</t>
+        </is>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -461,4 +466,72 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="256" style="0" width="12.856370192307693"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Not Sure</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Couldn't find it</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
+  <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="1" footer="1"/>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" fitToHeight="0" fitToWidth="0" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>